<commit_message>
start refactoring CalibraCurve into an R package
</commit_message>
<xml_diff>
--- a/example_data/ALB_LVNEVTEFAK_y8.xlsx
+++ b/example_data/ALB_LVNEVTEFAK_y8.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yan_farba/Studyproject/StuPro_SS24_CalibraCurve/example_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schorkka\Documents\UNI2\Projekte\CalibraCurve\CalibraCurve\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{56B2CB63-94F8-D64E-B15C-D316C14E5140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C710136-332F-49B7-90D2-5F5166C9C262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16000"/>
+    <workbookView xWindow="40750" yWindow="1390" windowWidth="28800" windowHeight="15370" xr2:uid="{8EDE7357-A882-441D-B364-3FDDA1B43071}"/>
   </bookViews>
   <sheets>
     <sheet name="ALB_LVNEVTEFAK_y8" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="112" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
   <si>
     <t>Protein</t>
   </si>
@@ -57,263 +52,161 @@
     <t>L1</t>
   </si>
   <si>
-    <t>7.5863448</t>
-  </si>
-  <si>
-    <t>6.51E-06</t>
-  </si>
-  <si>
-    <t>1.12E-05</t>
-  </si>
-  <si>
-    <t>4.30E-06</t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
-    <t>75.863448</t>
-  </si>
-  <si>
-    <t>0.000101611</t>
-  </si>
-  <si>
-    <t>8.85E-05</t>
-  </si>
-  <si>
-    <t>9.98E-05</t>
-  </si>
-  <si>
     <t>L3</t>
   </si>
   <si>
-    <t>758.63448</t>
-  </si>
-  <si>
-    <t>0.000913671</t>
-  </si>
-  <si>
-    <t>0.000932707</t>
-  </si>
-  <si>
-    <t>0.000937853</t>
-  </si>
-  <si>
     <t>L4</t>
   </si>
   <si>
-    <t>3793.1724</t>
-  </si>
-  <si>
-    <t>0.00540359</t>
-  </si>
-  <si>
-    <t>0.005493478</t>
-  </si>
-  <si>
-    <t>0.00539845</t>
-  </si>
-  <si>
     <t>L5</t>
   </si>
   <si>
-    <t>7586.3448</t>
-  </si>
-  <si>
-    <t>0.011693133</t>
-  </si>
-  <si>
-    <t>0.011529987</t>
-  </si>
-  <si>
-    <t>0.011493458</t>
-  </si>
-  <si>
     <t>L6</t>
   </si>
   <si>
-    <t>37931.724</t>
-  </si>
-  <si>
-    <t>0.069232899</t>
-  </si>
-  <si>
-    <t>0.068192386</t>
-  </si>
-  <si>
-    <t>0.07261995</t>
-  </si>
-  <si>
     <t>L7</t>
-  </si>
-  <si>
-    <t>75863.448</t>
-  </si>
-  <si>
-    <t>0.146624397</t>
-  </si>
-  <si>
-    <t>0.149734487</t>
-  </si>
-  <si>
-    <t>0.144802306</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -500,15 +393,15 @@
   </fills>
   <borders count="10">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -516,8 +409,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -525,8 +418,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -534,12 +427,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF7F7F7F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -549,12 +442,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -564,8 +457,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -573,12 +466,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="double">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="double">
+      </left>
+      <right style="double">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -588,12 +481,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FFB2B2B2"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -603,8 +496,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -658,52 +551,53 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -719,9 +613,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -729,39 +623,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -813,7 +707,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -865,32 +759,32 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110%"/>
-                <a:satMod val="105%"/>
-                <a:tint val="67%"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="103%"/>
-                <a:tint val="73%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="109%"/>
-                <a:tint val="81%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -898,25 +792,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103%"/>
-                <a:lumMod val="102%"/>
-                <a:tint val="94%"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110%"/>
-                <a:lumMod val="100%"/>
-                <a:shade val="100%"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99%"/>
-                <a:satMod val="120%"/>
-                <a:shade val="78%"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -924,26 +818,26 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -957,7 +851,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63%"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -969,32 +863,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95%"/>
-            <a:satMod val="170%"/>
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93%"/>
-                <a:satMod val="150%"/>
-                <a:shade val="98%"/>
-                <a:lumMod val="102%"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="98%"/>
-                <a:satMod val="130%"/>
-                <a:shade val="90%"/>
-                <a:lumMod val="103%"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63%"/>
-                <a:satMod val="120%"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1003,27 +897,47 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E9C0DA-D199-432D-ADAD-1F7E542CF78C}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1062,14 +976,14 @@
       <c r="E2">
         <v>51735624</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>7.5863448</v>
+      </c>
+      <c r="G2" s="1">
+        <v>6.5100000000000004E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1085,14 +999,14 @@
       <c r="E3">
         <v>25963551</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>7.5863448</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.1199999999999999E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1108,22 +1022,22 @@
       <c r="E4">
         <v>23943808</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>7.5863448</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4.3000000000000003E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
       <c r="D5">
         <v>3497</v>
@@ -1131,14 +1045,14 @@
       <c r="E5">
         <v>34415531</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>75.863448000000005</v>
+      </c>
+      <c r="G5">
+        <v>1.01611E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1146,7 +1060,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>1789</v>
@@ -1154,14 +1068,14 @@
       <c r="E6">
         <v>20219621</v>
       </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>75.863448000000005</v>
+      </c>
+      <c r="G6" s="1">
+        <v>8.8499999999999996E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1169,7 +1083,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>1738</v>
@@ -1177,14 +1091,14 @@
       <c r="E7">
         <v>17406861</v>
       </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>75.863448000000005</v>
+      </c>
+      <c r="G7" s="1">
+        <v>9.98E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1192,7 +1106,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>27649</v>
@@ -1200,14 +1114,14 @@
       <c r="E8">
         <v>30261442</v>
       </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>758.63448000000005</v>
+      </c>
+      <c r="G8">
+        <v>9.1367100000000001E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1215,7 +1129,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>16129</v>
@@ -1223,14 +1137,14 @@
       <c r="E9">
         <v>17292671</v>
       </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>758.63448000000005</v>
+      </c>
+      <c r="G9">
+        <v>9.3270699999999996E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1238,7 +1152,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>14648</v>
@@ -1246,14 +1160,14 @@
       <c r="E10">
         <v>15618645</v>
       </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>758.63448000000005</v>
+      </c>
+      <c r="G10">
+        <v>9.3785299999999999E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1175,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>147785</v>
@@ -1269,14 +1183,14 @@
       <c r="E11">
         <v>27349409</v>
       </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>3793.1723999999999</v>
+      </c>
+      <c r="G11">
+        <v>5.4035899999999998E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1284,7 +1198,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>90969</v>
@@ -1292,14 +1206,14 @@
       <c r="E12">
         <v>16559455</v>
       </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>3793.1723999999999</v>
+      </c>
+      <c r="G12">
+        <v>5.4934780000000004E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1221,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D13">
         <v>78851</v>
@@ -1315,14 +1229,14 @@
       <c r="E13">
         <v>14606229</v>
       </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>3793.1723999999999</v>
+      </c>
+      <c r="G13">
+        <v>5.39845E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1330,7 +1244,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>297396</v>
@@ -1338,14 +1252,14 @@
       <c r="E14">
         <v>25433389</v>
       </c>
-      <c r="F14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>7586.3447999999999</v>
+      </c>
+      <c r="G14">
+        <v>1.1693133E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1353,7 +1267,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>176654</v>
@@ -1361,14 +1275,14 @@
       <c r="E15">
         <v>15321266</v>
       </c>
-      <c r="F15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>7586.3447999999999</v>
+      </c>
+      <c r="G15">
+        <v>1.1529987E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1376,7 +1290,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>161072</v>
@@ -1384,14 +1298,14 @@
       <c r="E16">
         <v>14014233</v>
       </c>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>7586.3447999999999</v>
+      </c>
+      <c r="G16">
+        <v>1.1493458E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1313,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>1597763</v>
@@ -1407,14 +1321,14 @@
       <c r="E17">
         <v>23078089</v>
       </c>
-      <c r="F17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>37931.724000000002</v>
+      </c>
+      <c r="G17">
+        <v>6.9232899000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1422,7 +1336,7 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>925877</v>
@@ -1430,14 +1344,14 @@
       <c r="E18">
         <v>13577425</v>
       </c>
-      <c r="F18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>37931.724000000002</v>
+      </c>
+      <c r="G18">
+        <v>6.8192385999999994E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1445,7 +1359,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>873483</v>
@@ -1453,14 +1367,14 @@
       <c r="E19">
         <v>12028141</v>
       </c>
-      <c r="F19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>37931.724000000002</v>
+      </c>
+      <c r="G19">
+        <v>7.2619950000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1468,7 +1382,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D20">
         <v>2969849</v>
@@ -1476,14 +1390,14 @@
       <c r="E20">
         <v>20254808</v>
       </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>75863.448000000004</v>
+      </c>
+      <c r="G20">
+        <v>0.14662439699999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1491,7 +1405,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D21">
         <v>1883433</v>
@@ -1499,14 +1413,14 @@
       <c r="E21">
         <v>12578485</v>
       </c>
-      <c r="F21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>75863.448000000004</v>
+      </c>
+      <c r="G21">
+        <v>0.149734487</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +1428,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>1701122</v>
@@ -1522,14 +1436,14 @@
       <c r="E22">
         <v>11747893</v>
       </c>
-      <c r="F22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" t="s">
-        <v>43</v>
+      <c r="F22">
+        <v>75863.448000000004</v>
+      </c>
+      <c r="G22">
+        <v>0.14480230599999999</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>